<commit_message>
SingVacc TC7 e SingVacc TC9
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="146">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -810,6 +810,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.90.4.4.7cdbc659ade53971ad4fee9066fcfe3a58904f6ba03e60b8c047dec31464f0d0.665ebe046f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T16:06:35Z</t>
+  </si>
+  <si>
+    <t>f046ce26006388f5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.2c9edbff1c5a4a41649812981317b66b6f683d4683f03518063aebcbdc4dc5e4.3b26100e8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T16:19:54Z</t>
+  </si>
+  <si>
+    <t>f6b87b5563503880</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.9d44a696ce33f392062023517bd0fe90222b7d74cefa272e62b605b39228e6cd.b7ef544b68^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2688,7 +2706,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomRight" activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3771,13 +3789,23 @@
       <c r="E39" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
+      <c r="F39" s="20">
+        <v>44960</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="I39" s="21" t="s">
+        <v>142</v>
+      </c>
       <c r="J39" s="22"/>
       <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
+      <c r="L39" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="M39" s="22"/>
       <c r="N39" s="23" t="s">
         <v>47</v>
@@ -3805,7 +3833,9 @@
       <c r="H40" s="21"/>
       <c r="I40" s="21"/>
       <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
+      <c r="K40" s="22" t="s">
+        <v>124</v>
+      </c>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
       <c r="N40" s="23" t="s">
@@ -3829,13 +3859,23 @@
       <c r="E41" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
+      <c r="F41" s="20">
+        <v>44960</v>
+      </c>
+      <c r="G41" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="I41" s="21" t="s">
+        <v>145</v>
+      </c>
       <c r="J41" s="22"/>
       <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
+      <c r="L41" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="M41" s="22"/>
       <c r="N41" s="23" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
SingVacc TC11 e SingVacc TC13
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="152">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -837,6 +837,15 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.90.4.4.09eaeb541361fcd87e79fee58b997835fe42480f6547e0a02946bb186f9d02eb.4a98c497c0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-03T16:44:53Z</t>
+  </si>
+  <si>
+    <t>6b969dc0c80cdc5c</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.9b39b0966ba8b8371ac6d3cbeac80c930132404a0b392dbffa3e03a544f25462.1db38fca70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2712,10 +2721,10 @@
   <dimension ref="A1:O896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L42" sqref="L42"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3946,13 +3955,23 @@
       <c r="E43" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
+      <c r="F43" s="20">
+        <v>44960</v>
+      </c>
+      <c r="G43" s="21" t="s">
+        <v>149</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="I43" s="21" t="s">
+        <v>151</v>
+      </c>
       <c r="J43" s="22"/>
       <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
+      <c r="L43" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="M43" s="22"/>
       <c r="N43" s="23" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Corretto CertVacc TC3 inserita categoria di rischio nella somministrazione
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -911,13 +911,13 @@
     <t>2.16.840.1.113883.2.9.2.90.4.4.11cdc6d7029c467805ea83b5d928e53f2dfd876a74ccf257b77bb315a437305d.2ca2262a70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-02-07T10:21:15Z</t>
-  </si>
-  <si>
-    <t>ad92964cb65ce66c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.9f3473998ad23aaa26357b3c70430b4e49be42f18ba775573d4aa9bf5d076c6d.a186fa7896^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-02-07T10:37:44Z</t>
+  </si>
+  <si>
+    <t>6424e05331d59204</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.f7fbdb8518942fc7623480d4a9127da0e5129e690004c9564b7dd3f99f312b48.b0239a7138^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2796,7 +2796,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3087,7 +3087,7 @@
       <c r="G12" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="49" t="s">
         <v>174</v>
       </c>
       <c r="I12" s="21" t="s">

</xml_diff>

<commit_message>
CertVacc TC6 e C7
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="188">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -936,6 +936,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.90.4.4.a7c686cb97b6b996280eea8c2c140032a998fefa7ae27efb64ef70077ce8a222.f77e04ad19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1b1b7d45b912f42d</t>
+  </si>
+  <si>
+    <t>2023-02-07T11:28:47Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.86d5071b6dca0779ff83c8ad50036f11080594edf0ea7c4dc164a003f1e5c77a.ad767223a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-07T11:41:35Z</t>
+  </si>
+  <si>
+    <t>11b5209b37842e10</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.e748357fa64cbd1f05e0b8d703203d0aa65e1ac6877848f10c8668f1aaff247a.f78baeaba6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2811,20 +2829,21 @@
   <dimension ref="A1:O896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L18" sqref="L18"/>
+      <selection pane="bottomRight" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
-    <col min="6" max="9" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+    <col min="7" max="9" width="33.28515625" customWidth="1"/>
     <col min="10" max="11" width="27.28515625" customWidth="1"/>
     <col min="12" max="12" width="33.28515625" customWidth="1"/>
     <col min="13" max="13" width="36.42578125" customWidth="1"/>
@@ -3009,7 +3028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="246" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
         <v>16</v>
       </c>
@@ -3046,7 +3065,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="24"/>
     </row>
-    <row r="11" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="241.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
         <v>17</v>
       </c>
@@ -3083,7 +3102,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="24"/>
     </row>
-    <row r="12" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="186" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <v>18</v>
       </c>
@@ -3120,7 +3139,7 @@
       <c r="N12" s="23"/>
       <c r="O12" s="24"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="141.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
         <v>19</v>
       </c>
@@ -3157,7 +3176,7 @@
       <c r="N13" s="23"/>
       <c r="O13" s="24"/>
     </row>
-    <row r="14" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
         <v>20</v>
       </c>
@@ -3194,7 +3213,7 @@
       <c r="N14" s="23"/>
       <c r="O14" s="24"/>
     </row>
-    <row r="15" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="214.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17">
         <v>21</v>
       </c>
@@ -3231,7 +3250,7 @@
       <c r="N15" s="23"/>
       <c r="O15" s="24"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="206.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17">
         <v>22</v>
       </c>
@@ -3258,7 +3277,7 @@
       <c r="N16" s="23"/>
       <c r="O16" s="24"/>
     </row>
-    <row r="17" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="286.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17">
         <v>23</v>
       </c>
@@ -3295,7 +3314,7 @@
       <c r="N17" s="23"/>
       <c r="O17" s="24"/>
     </row>
-    <row r="18" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="192" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>33</v>
       </c>
@@ -3334,7 +3353,7 @@
       </c>
       <c r="O18" s="24"/>
     </row>
-    <row r="19" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="195" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>34</v>
       </c>
@@ -3363,7 +3382,7 @@
       </c>
       <c r="O19" s="24"/>
     </row>
-    <row r="20" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="193.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>41</v>
       </c>
@@ -3392,7 +3411,7 @@
       </c>
       <c r="O20" s="24"/>
     </row>
-    <row r="21" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="173.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17">
         <v>42</v>
       </c>
@@ -3421,7 +3440,7 @@
       </c>
       <c r="O21" s="24"/>
     </row>
-    <row r="22" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17">
         <v>49</v>
       </c>
@@ -3450,7 +3469,7 @@
       </c>
       <c r="O22" s="24"/>
     </row>
-    <row r="23" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="86.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>50</v>
       </c>
@@ -3479,7 +3498,7 @@
       </c>
       <c r="O23" s="24"/>
     </row>
-    <row r="24" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17">
         <v>94</v>
       </c>
@@ -3495,13 +3514,23 @@
       <c r="E24" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="F24" s="20">
+        <v>44964</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>181</v>
+      </c>
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
+      <c r="L24" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="M24" s="22"/>
       <c r="N24" s="23" t="s">
         <v>47</v>
@@ -3524,13 +3553,23 @@
       <c r="E25" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
+      <c r="F25" s="20">
+        <v>44964</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>184</v>
+      </c>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
+      <c r="L25" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="M25" s="22"/>
       <c r="N25" s="23" t="s">
         <v>47</v>
@@ -3553,20 +3592,30 @@
       <c r="E26" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="F26" s="20">
+        <v>44964</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>187</v>
+      </c>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
+      <c r="L26" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="M26" s="22"/>
       <c r="N26" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O26" s="24"/>
     </row>
-    <row r="27" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="207" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>97</v>
       </c>
@@ -3595,7 +3644,7 @@
       </c>
       <c r="O27" s="24"/>
     </row>
-    <row r="28" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>98</v>
       </c>
@@ -3621,7 +3670,7 @@
       </c>
       <c r="O28" s="24"/>
     </row>
-    <row r="29" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="217.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>99</v>
       </c>
@@ -3650,7 +3699,7 @@
       </c>
       <c r="O29" s="24"/>
     </row>
-    <row r="30" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="17">
         <v>100</v>
       </c>
@@ -3679,7 +3728,7 @@
       </c>
       <c r="O30" s="24"/>
     </row>
-    <row r="31" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="201.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17">
         <v>101</v>
       </c>
@@ -3737,7 +3786,7 @@
       </c>
       <c r="O32" s="24"/>
     </row>
-    <row r="33" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="17">
         <v>103</v>
       </c>
@@ -3766,7 +3815,7 @@
       </c>
       <c r="O33" s="24"/>
     </row>
-    <row r="34" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>104</v>
       </c>
@@ -3795,7 +3844,7 @@
       </c>
       <c r="O34" s="24"/>
     </row>
-    <row r="35" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="183" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>105</v>
       </c>
@@ -3824,7 +3873,7 @@
       </c>
       <c r="O35" s="24"/>
     </row>
-    <row r="36" spans="1:15" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="198.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>106</v>
       </c>
@@ -3853,7 +3902,7 @@
       </c>
       <c r="O36" s="24"/>
     </row>
-    <row r="37" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="17">
         <v>107</v>
       </c>
@@ -3892,7 +3941,7 @@
       </c>
       <c r="O37" s="24"/>
     </row>
-    <row r="38" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17">
         <v>108</v>
       </c>
@@ -3931,7 +3980,7 @@
       </c>
       <c r="O38" s="24"/>
     </row>
-    <row r="39" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="100.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
         <v>109</v>
       </c>
@@ -3970,7 +4019,7 @@
       </c>
       <c r="O39" s="24"/>
     </row>
-    <row r="40" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="185.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17">
         <v>110</v>
       </c>
@@ -4001,7 +4050,7 @@
       </c>
       <c r="O40" s="24"/>
     </row>
-    <row r="41" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="191.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17">
         <v>111</v>
       </c>
@@ -4040,7 +4089,7 @@
       </c>
       <c r="O41" s="24"/>
     </row>
-    <row r="42" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="94.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>112</v>
       </c>
@@ -4079,7 +4128,7 @@
       </c>
       <c r="O42" s="24"/>
     </row>
-    <row r="43" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="186" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>113</v>
       </c>
@@ -4118,7 +4167,7 @@
       </c>
       <c r="O43" s="24"/>
     </row>
-    <row r="44" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="198" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>114</v>
       </c>
@@ -4147,7 +4196,7 @@
       </c>
       <c r="O44" s="24"/>
     </row>
-    <row r="45" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="183.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>115</v>
       </c>
@@ -4186,7 +4235,7 @@
       </c>
       <c r="O45" s="24"/>
     </row>
-    <row r="46" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="179.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17">
         <v>116</v>
       </c>
@@ -4225,7 +4274,7 @@
       </c>
       <c r="O46" s="24"/>
     </row>
-    <row r="47" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="203.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17">
         <v>117</v>
       </c>
@@ -4264,7 +4313,7 @@
       </c>
       <c r="O47" s="24"/>
     </row>
-    <row r="48" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="180" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="17">
         <v>118</v>
       </c>
@@ -4303,7 +4352,7 @@
       </c>
       <c r="O48" s="24"/>
     </row>
-    <row r="49" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="180.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="17">
         <v>119</v>
       </c>
@@ -4342,7 +4391,7 @@
       </c>
       <c r="O49" s="24"/>
     </row>
-    <row r="50" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="182.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>120</v>
       </c>
@@ -4371,7 +4420,7 @@
       </c>
       <c r="O50" s="24"/>
     </row>
-    <row r="51" spans="1:15" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="177.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>121</v>
       </c>

</xml_diff>

<commit_message>
CertVacc TC10 e TC11
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="197">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -963,6 +963,24 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.90.4.4.cbd8ff5df29e9695698a48e30238833eb1bcfb7c270dd6f644a986ee69633eb7.67b4ef962b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-07T11:53:19Z</t>
+  </si>
+  <si>
+    <t>cae0f57af9a87c4b</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.35580b5b865075ce4d136f0b375c8f7bc347988c72705d47abe7ec7e242b1519.f74023dd4d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-02-07T11:58:35Z</t>
+  </si>
+  <si>
+    <t>443c12fb7af75190</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.c030383685a4f8cb08aa6e28c5cb80fe3f38692de2498b9d72376a214e56c87c.c3c2261e28^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -1057,7 +1075,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1316,19 +1334,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -1407,7 +1412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1492,15 +1497,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1533,22 +1538,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2919,10 +2921,10 @@
   <dimension ref="A1:O896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
+      <selection pane="bottomRight" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3755,10 +3757,10 @@
       <c r="F28" s="20">
         <v>44964</v>
       </c>
-      <c r="G28" s="56" t="s">
+      <c r="G28" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="H28" s="56" t="s">
+      <c r="H28" s="55" t="s">
         <v>188</v>
       </c>
       <c r="I28" s="51" t="s">
@@ -3791,20 +3793,30 @@
       <c r="E29" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="54"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="21"/>
+      <c r="F29" s="20">
+        <v>44964</v>
+      </c>
+      <c r="G29" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="H29" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="I29" s="21" t="s">
+        <v>193</v>
+      </c>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
+      <c r="L29" s="22" t="s">
+        <v>123</v>
+      </c>
       <c r="M29" s="22"/>
       <c r="N29" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O29" s="24"/>
     </row>
-    <row r="30" spans="1:15" ht="202.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="202.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>100</v>
       </c>
@@ -3820,10 +3832,18 @@
       <c r="E30" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
+      <c r="F30" s="20">
+        <v>44964</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="I30" s="21" t="s">
+        <v>196</v>
+      </c>
       <c r="J30" s="22"/>
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
@@ -3833,7 +3853,7 @@
       </c>
       <c r="O30" s="24"/>
     </row>
-    <row r="31" spans="1:15" ht="201.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="201.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Restano vuori solo i TC relativi all'issue https://github.com/ministero-salute/it-fse-support/issues/88
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="225">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -3005,10 +3005,10 @@
   <dimension ref="A1:O896"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L50" sqref="L50"/>
+      <selection pane="bottomRight" activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4495,7 +4495,9 @@
       <c r="H44" s="21"/>
       <c r="I44" s="21"/>
       <c r="J44" s="22"/>
-      <c r="K44" s="22"/>
+      <c r="K44" s="22" t="s">
+        <v>124</v>
+      </c>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
       <c r="N44" s="23" t="s">
@@ -4745,7 +4747,9 @@
       <c r="E51" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F51" s="20"/>
+      <c r="F51" s="20" t="s">
+        <v>221</v>
+      </c>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
       <c r="I51" s="21"/>

</xml_diff>

<commit_message>
Adeguamenti richiesti mail ministero del 14/02
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="188">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -793,69 +793,6 @@
     <t>2.16.840.1.113883.2.9.2.90.4.4.41309ad9ee4a4dc5d8d043451d8fd76972699d3f573504fe5a355b3cfe1feb28.91a491e549^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-02-03T15:59:31Z</t>
-  </si>
-  <si>
-    <t>0707fbe98f8267c9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.7cdbc659ade53971ad4fee9066fcfe3a58904f6ba03e60b8c047dec31464f0d0.665ebe046f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T16:06:35Z</t>
-  </si>
-  <si>
-    <t>f046ce26006388f5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.2c9edbff1c5a4a41649812981317b66b6f683d4683f03518063aebcbdc4dc5e4.3b26100e8d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T16:19:54Z</t>
-  </si>
-  <si>
-    <t>f6b87b5563503880</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.9d44a696ce33f392062023517bd0fe90222b7d74cefa272e62b605b39228e6cd.b7ef544b68^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T16:28:04Z</t>
-  </si>
-  <si>
-    <t>8e12c64f320df259</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.09eaeb541361fcd87e79fee58b997835fe42480f6547e0a02946bb186f9d02eb.4a98c497c0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T16:44:53Z</t>
-  </si>
-  <si>
-    <t>6b969dc0c80cdc5c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.9b39b0966ba8b8371ac6d3cbeac80c930132404a0b392dbffa3e03a544f25462.1db38fca70^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T16:53:54Z</t>
-  </si>
-  <si>
-    <t>3da65d831debea49</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.1d9abba9b315b3df3fd3d1da830b2c6ccd8d07c703dd14dac922133de4858246.383cbac1a7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-03T17:01:25Z</t>
-  </si>
-  <si>
-    <t>d8247cc017c6a1ac</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.056ddf47f7a1b991b2da72a001d39e3b230b164a9b987e0608181ca52b47041b.ba479a7a06^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-02-03T17:10:51Z</t>
   </si>
   <si>
@@ -919,60 +856,6 @@
     <t>2.16.840.1.113883.2.9.2.90.4.4.a7c686cb97b6b996280eea8c2c140032a998fefa7ae27efb64ef70077ce8a222.f77e04ad19^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>1b1b7d45b912f42d</t>
-  </si>
-  <si>
-    <t>2023-02-07T11:28:47Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.86d5071b6dca0779ff83c8ad50036f11080594edf0ea7c4dc164a003f1e5c77a.ad767223a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-07T11:41:35Z</t>
-  </si>
-  <si>
-    <t>11b5209b37842e10</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.e748357fa64cbd1f05e0b8d703203d0aa65e1ac6877848f10c8668f1aaff247a.f78baeaba6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>d117d2bc3216f1d0</t>
-  </si>
-  <si>
-    <t>2023-02-07T11:49:03Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.cbd8ff5df29e9695698a48e30238833eb1bcfb7c270dd6f644a986ee69633eb7.67b4ef962b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-07T11:53:19Z</t>
-  </si>
-  <si>
-    <t>cae0f57af9a87c4b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.35580b5b865075ce4d136f0b375c8f7bc347988c72705d47abe7ec7e242b1519.f74023dd4d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-07T11:58:35Z</t>
-  </si>
-  <si>
-    <t>443c12fb7af75190</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.c030383685a4f8cb08aa6e28c5cb80fe3f38692de2498b9d72376a214e56c87c.c3c2261e28^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-07T12:04:00Z</t>
-  </si>
-  <si>
-    <t>817f7181858d32c8</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.e3e700a36a8a8895d6f1fc6fc9fe2b78ff34549bdf0ab1b39f5573f85fb1466d.359060711c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>80d66f45c9200b0b</t>
   </si>
   <si>
@@ -1000,24 +883,6 @@
     <t>2.16.840.1.113883.2.9.2.90.4.4.98a44413ac3e3e63ad292e49a394f2bba8c549459076c22c8eb7b48cf382f489.8ce342cdf8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-02-07T13:49:58Z</t>
-  </si>
-  <si>
-    <t>e15a84008f005021</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.34b4b527d2bfc15fb2283dad296350086254f08f27bf2923e81c4cf7a00c4e15.c3afee8a16^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-07T14:45:21Z</t>
-  </si>
-  <si>
-    <t>a9d8d37d5f859514</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.9f916df79284a8bc7af5ec232106c389fd37c275be24e9107b7dc529eb9289eb.7676c86162^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-02-07T14:55:32Z</t>
   </si>
   <si>
@@ -1046,15 +911,6 @@
   </si>
   <si>
     <t>In attesa correzione bug GW: https://github.com/ministero-salute/it-fse-support/issues/88</t>
-  </si>
-  <si>
-    <t>659e029a5c09a75d</t>
-  </si>
-  <si>
-    <t>2023-02-07T15:51:09</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.ac8a25e009f59c6ad4b774d2ee67500920982516f4c0cb8c9d96cb9621a8061a.21b439bce6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>L'errore a regime non si presenterà: facciamo preventivamente l'uppercase del CF</t>
@@ -3026,11 +2882,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O896"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B47" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="H48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A51" sqref="A51"/>
+      <selection pane="bottomRight" activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3246,13 +3102,13 @@
         <v>44963</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
@@ -3283,13 +3139,13 @@
         <v>44963</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="I11" s="21" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
@@ -3320,13 +3176,13 @@
         <v>44964</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
@@ -3357,13 +3213,13 @@
         <v>44964</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>175</v>
+        <v>154</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
@@ -3476,7 +3332,7 @@
       <c r="M16" s="22"/>
       <c r="N16" s="23"/>
       <c r="O16" s="20" t="s">
-        <v>234</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3536,21 +3392,19 @@
         <v>44964</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="I18" s="21" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="J18" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K18" s="22"/>
-      <c r="L18" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L18" s="22"/>
       <c r="M18" s="22"/>
       <c r="N18" s="23" t="s">
         <v>47</v>
@@ -3577,21 +3431,19 @@
         <v>44964</v>
       </c>
       <c r="G19" s="21" t="s">
-        <v>217</v>
+        <v>172</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>216</v>
+        <v>171</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K19" s="22"/>
-      <c r="L19" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L19" s="22"/>
       <c r="M19" s="22"/>
       <c r="N19" s="23" t="s">
         <v>47</v>
@@ -3618,16 +3470,16 @@
         <v>44964</v>
       </c>
       <c r="G20" s="21" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>213</v>
+        <v>168</v>
       </c>
       <c r="I20" s="21" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
@@ -3657,16 +3509,16 @@
         <v>44964</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>219</v>
+        <v>174</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>218</v>
+        <v>173</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K21" s="22"/>
       <c r="L21" s="22"/>
@@ -3699,7 +3551,7 @@
       <c r="H22" s="21"/>
       <c r="I22" s="21"/>
       <c r="J22" s="22" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="K22" s="22"/>
       <c r="L22" s="22"/>
@@ -3732,7 +3584,7 @@
       <c r="H23" s="21"/>
       <c r="I23" s="21"/>
       <c r="J23" s="22" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="K23" s="22"/>
       <c r="L23" s="22"/>
@@ -3762,21 +3614,19 @@
         <v>44964</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>177</v>
+        <v>156</v>
       </c>
       <c r="H24" s="21" t="s">
-        <v>176</v>
+        <v>155</v>
       </c>
       <c r="I24" s="21" t="s">
-        <v>178</v>
+        <v>157</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K24" s="22"/>
-      <c r="L24" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L24" s="22"/>
       <c r="M24" s="22"/>
       <c r="N24" s="23" t="s">
         <v>47</v>
@@ -3799,31 +3649,21 @@
       <c r="E25" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F25" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>180</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="I25" s="21" t="s">
-        <v>181</v>
-      </c>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
       <c r="J25" s="22"/>
       <c r="K25" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L25" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L25" s="22"/>
       <c r="M25" s="22"/>
       <c r="N25" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O25" s="24" t="s">
-        <v>225</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3842,31 +3682,21 @@
       <c r="E26" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G26" s="41" t="s">
-        <v>182</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>183</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>184</v>
-      </c>
+      <c r="F26" s="20"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="22"/>
       <c r="K26" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L26" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L26" s="22"/>
       <c r="M26" s="22"/>
       <c r="N26" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O26" s="24" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3916,31 +3746,21 @@
       <c r="E28" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F28" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G28" s="43" t="s">
-        <v>186</v>
-      </c>
-      <c r="H28" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="I28" s="39" t="s">
-        <v>187</v>
-      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="39"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L28" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L28" s="22"/>
       <c r="M28" s="22"/>
       <c r="N28" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O28" s="24" t="s">
-        <v>233</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="118.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3959,31 +3779,21 @@
       <c r="E29" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>188</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>189</v>
-      </c>
-      <c r="I29" s="21" t="s">
-        <v>190</v>
-      </c>
+      <c r="F29" s="20"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L29" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L29" s="22"/>
       <c r="M29" s="22"/>
       <c r="N29" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O29" s="24" t="s">
-        <v>230</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4002,18 +3812,10 @@
       <c r="E30" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G30" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="H30" s="21" t="s">
-        <v>192</v>
-      </c>
-      <c r="I30" s="21" t="s">
-        <v>193</v>
-      </c>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="22"/>
       <c r="K30" s="22" t="s">
         <v>124</v>
@@ -4024,7 +3826,7 @@
         <v>47</v>
       </c>
       <c r="O30" s="24" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4043,31 +3845,21 @@
       <c r="E31" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>194</v>
-      </c>
-      <c r="H31" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="I31" s="21" t="s">
-        <v>196</v>
-      </c>
+      <c r="F31" s="20"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="22"/>
       <c r="K31" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L31" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L31" s="22"/>
       <c r="M31" s="22"/>
       <c r="N31" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O31" s="24" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4090,21 +3882,19 @@
         <v>44964</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>198</v>
+        <v>159</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>199</v>
+        <v>160</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K32" s="22"/>
-      <c r="L32" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L32" s="22"/>
       <c r="M32" s="22"/>
       <c r="N32" s="23" t="s">
         <v>47</v>
@@ -4131,21 +3921,19 @@
         <v>44964</v>
       </c>
       <c r="G33" s="21" t="s">
-        <v>200</v>
+        <v>161</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>202</v>
+        <v>163</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K33" s="22"/>
-      <c r="L33" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L33" s="22"/>
       <c r="M33" s="22"/>
       <c r="N33" s="23" t="s">
         <v>47</v>
@@ -4172,21 +3960,19 @@
         <v>44964</v>
       </c>
       <c r="G34" s="21" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>203</v>
+        <v>164</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>205</v>
+        <v>166</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K34" s="22"/>
-      <c r="L34" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L34" s="22"/>
       <c r="M34" s="22"/>
       <c r="N34" s="23" t="s">
         <v>47</v>
@@ -4209,31 +3995,21 @@
       <c r="E35" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F35" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G35" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="I35" s="21" t="s">
-        <v>208</v>
-      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
       <c r="J35" s="22"/>
       <c r="K35" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L35" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L35" s="22"/>
       <c r="M35" s="22"/>
       <c r="N35" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O35" s="24" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4252,31 +4028,21 @@
       <c r="E36" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F36" s="20">
-        <v>44964</v>
-      </c>
-      <c r="G36" s="21" t="s">
-        <v>209</v>
-      </c>
-      <c r="H36" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="I36" s="21" t="s">
-        <v>211</v>
-      </c>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
       <c r="J36" s="22"/>
       <c r="K36" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L36" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L36" s="22"/>
       <c r="M36" s="22"/>
       <c r="N36" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O36" s="24" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4308,12 +4074,10 @@
         <v>136</v>
       </c>
       <c r="J37" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K37" s="22"/>
-      <c r="L37" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L37" s="22"/>
       <c r="M37" s="22"/>
       <c r="N37" s="23" t="s">
         <v>47</v>
@@ -4336,31 +4100,21 @@
       <c r="E38" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="F38" s="20">
-        <v>44960</v>
-      </c>
-      <c r="G38" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>139</v>
-      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
       <c r="J38" s="22"/>
       <c r="K38" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L38" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L38" s="22"/>
       <c r="M38" s="22"/>
       <c r="N38" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O38" s="24" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4379,31 +4133,21 @@
       <c r="E39" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="F39" s="20">
-        <v>44960</v>
-      </c>
-      <c r="G39" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>141</v>
-      </c>
-      <c r="I39" s="21" t="s">
-        <v>142</v>
-      </c>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
       <c r="J39" s="22"/>
       <c r="K39" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L39" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L39" s="22"/>
       <c r="M39" s="22"/>
       <c r="N39" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O39" s="24" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4422,9 +4166,7 @@
       <c r="E40" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="F40" s="20">
-        <v>44960</v>
-      </c>
+      <c r="F40" s="20"/>
       <c r="G40" s="21"/>
       <c r="H40" s="21"/>
       <c r="I40" s="21"/>
@@ -4455,31 +4197,21 @@
       <c r="E41" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="20">
-        <v>44960</v>
-      </c>
-      <c r="G41" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="H41" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="I41" s="21" t="s">
-        <v>145</v>
-      </c>
+      <c r="F41" s="20"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
       <c r="J41" s="22"/>
       <c r="K41" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L41" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L41" s="22"/>
       <c r="M41" s="22"/>
       <c r="N41" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O41" s="24" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4498,31 +4230,21 @@
       <c r="E42" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="F42" s="20">
-        <v>44960</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="H42" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>148</v>
-      </c>
+      <c r="F42" s="20"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
       <c r="J42" s="22"/>
       <c r="K42" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L42" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L42" s="22"/>
       <c r="M42" s="22"/>
       <c r="N42" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O42" s="24" t="s">
-        <v>230</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4541,31 +4263,21 @@
       <c r="E43" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="F43" s="20">
-        <v>44960</v>
-      </c>
-      <c r="G43" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="H43" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="I43" s="21" t="s">
-        <v>151</v>
-      </c>
+      <c r="F43" s="20"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
       <c r="J43" s="22"/>
       <c r="K43" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L43" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L43" s="22"/>
       <c r="M43" s="22"/>
       <c r="N43" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O43" s="24" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4598,7 +4310,7 @@
         <v>47</v>
       </c>
       <c r="O44" s="24" t="s">
-        <v>231</v>
+        <v>183</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4617,31 +4329,21 @@
       <c r="E45" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F45" s="20">
-        <v>44960</v>
-      </c>
-      <c r="G45" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="H45" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="I45" s="21" t="s">
-        <v>154</v>
-      </c>
+      <c r="F45" s="20"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
       <c r="J45" s="22"/>
       <c r="K45" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L45" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L45" s="22"/>
       <c r="M45" s="22"/>
       <c r="N45" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O45" s="24" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4660,31 +4362,21 @@
       <c r="E46" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="F46" s="20">
-        <v>44960</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="H46" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="I46" s="21" t="s">
-        <v>157</v>
-      </c>
+      <c r="F46" s="20"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
       <c r="J46" s="22"/>
       <c r="K46" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L46" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L46" s="22"/>
       <c r="M46" s="22"/>
       <c r="N46" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O46" s="24" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4707,21 +4399,19 @@
         <v>44960</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="H47" s="21" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="I47" s="21" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K47" s="22"/>
-      <c r="L47" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L47" s="22"/>
       <c r="M47" s="22"/>
       <c r="N47" s="23" t="s">
         <v>47</v>
@@ -4748,21 +4438,19 @@
         <v>44963</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="H48" s="21" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="I48" s="21" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="J48" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K48" s="22"/>
-      <c r="L48" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L48" s="22"/>
       <c r="M48" s="22"/>
       <c r="N48" s="23" t="s">
         <v>47</v>
@@ -4799,7 +4487,7 @@
         <v>47</v>
       </c>
       <c r="O49" s="24" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4821,28 +4509,20 @@
       <c r="F50" s="20">
         <v>44964</v>
       </c>
-      <c r="G50" s="21" t="s">
-        <v>223</v>
-      </c>
-      <c r="H50" s="21" t="s">
-        <v>222</v>
-      </c>
-      <c r="I50" s="21" t="s">
-        <v>224</v>
-      </c>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
       <c r="J50" s="22"/>
       <c r="K50" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="L50" s="22" t="s">
-        <v>123</v>
-      </c>
+      <c r="L50" s="22"/>
       <c r="M50" s="22"/>
       <c r="N50" s="23" t="s">
         <v>47</v>
       </c>
       <c r="O50" s="24" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4862,13 +4542,13 @@
         <v>114</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>221</v>
+        <v>176</v>
       </c>
       <c r="G51" s="21"/>
       <c r="H51" s="21"/>
       <c r="I51" s="21"/>
       <c r="J51" s="22" t="s">
-        <v>235</v>
+        <v>187</v>
       </c>
       <c r="K51" s="22"/>
       <c r="L51" s="22"/>

</xml_diff>

<commit_message>
Adeguamenti richiesti tramite mail oggi da fse_support@sogei.it
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist_V4.1.xlsx
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="194">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -956,6 +956,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.90.4.4.21b4a6d4582e24e59a93e58b02d7ebb369c2a92f78e2e4239541bddbbe73b2c6.27e3fb0981^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Il campo indirizzo non risulta valorizzato</t>
+  </si>
+  <si>
+    <t>Il campo indirizzo non è valorizzato</t>
   </si>
 </sst>
 </file>
@@ -2898,7 +2904,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="F45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="J51" sqref="J51"/>
+      <selection pane="bottomRight" activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3422,7 +3428,9 @@
         <v>185</v>
       </c>
       <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
+      <c r="L18" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M18" s="22"/>
       <c r="N18" s="23" t="s">
         <v>47</v>
@@ -3461,7 +3469,9 @@
         <v>185</v>
       </c>
       <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
+      <c r="L19" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M19" s="22"/>
       <c r="N19" s="23" t="s">
         <v>47</v>
@@ -3500,7 +3510,9 @@
         <v>185</v>
       </c>
       <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
+      <c r="L20" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M20" s="22"/>
       <c r="N20" s="23" t="s">
         <v>47</v>
@@ -3539,7 +3551,9 @@
         <v>185</v>
       </c>
       <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
+      <c r="L21" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M21" s="22"/>
       <c r="N21" s="23" t="s">
         <v>47</v>
@@ -3572,7 +3586,9 @@
         <v>170</v>
       </c>
       <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
+      <c r="L22" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M22" s="22"/>
       <c r="N22" s="23" t="s">
         <v>47</v>
@@ -3605,7 +3621,9 @@
         <v>170</v>
       </c>
       <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
+      <c r="L23" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M23" s="22"/>
       <c r="N23" s="23" t="s">
         <v>47</v>
@@ -3644,7 +3662,9 @@
         <v>185</v>
       </c>
       <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
+      <c r="L24" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M24" s="22"/>
       <c r="N24" s="23" t="s">
         <v>47</v>
@@ -3676,13 +3696,13 @@
         <v>124</v>
       </c>
       <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
+      <c r="M25" s="22" t="s">
+        <v>176</v>
+      </c>
       <c r="N25" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O25" s="24" t="s">
-        <v>176</v>
-      </c>
+      <c r="O25" s="24"/>
     </row>
     <row r="26" spans="1:15" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
@@ -3709,13 +3729,13 @@
         <v>124</v>
       </c>
       <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
+      <c r="M26" s="22" t="s">
+        <v>179</v>
+      </c>
       <c r="N26" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O26" s="24" t="s">
-        <v>179</v>
-      </c>
+      <c r="O26" s="24"/>
     </row>
     <row r="27" spans="1:15" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
@@ -3742,7 +3762,9 @@
         <v>124</v>
       </c>
       <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
+      <c r="M27" s="22" t="s">
+        <v>192</v>
+      </c>
       <c r="N27" s="23" t="s">
         <v>47</v>
       </c>
@@ -3773,13 +3795,13 @@
         <v>124</v>
       </c>
       <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
+      <c r="M28" s="22" t="s">
+        <v>184</v>
+      </c>
       <c r="N28" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O28" s="24" t="s">
-        <v>184</v>
-      </c>
+      <c r="O28" s="24"/>
     </row>
     <row r="29" spans="1:15" ht="118.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
@@ -3806,13 +3828,13 @@
         <v>124</v>
       </c>
       <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
+      <c r="M29" s="22" t="s">
+        <v>181</v>
+      </c>
       <c r="N29" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O29" s="24" t="s">
-        <v>181</v>
-      </c>
+      <c r="O29" s="24"/>
     </row>
     <row r="30" spans="1:15" ht="82.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
@@ -3839,13 +3861,13 @@
         <v>124</v>
       </c>
       <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
+      <c r="M30" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="N30" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O30" s="24" t="s">
-        <v>177</v>
-      </c>
+      <c r="O30" s="24"/>
     </row>
     <row r="31" spans="1:15" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
@@ -3872,13 +3894,13 @@
         <v>124</v>
       </c>
       <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
+      <c r="M31" s="22" t="s">
+        <v>183</v>
+      </c>
       <c r="N31" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O31" s="24" t="s">
-        <v>183</v>
-      </c>
+      <c r="O31" s="24"/>
     </row>
     <row r="32" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
@@ -3912,7 +3934,9 @@
         <v>185</v>
       </c>
       <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
+      <c r="L32" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M32" s="22"/>
       <c r="N32" s="23" t="s">
         <v>47</v>
@@ -3951,7 +3975,9 @@
         <v>185</v>
       </c>
       <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
+      <c r="L33" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M33" s="22"/>
       <c r="N33" s="23" t="s">
         <v>47</v>
@@ -3990,7 +4016,9 @@
         <v>185</v>
       </c>
       <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
+      <c r="L34" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M34" s="22"/>
       <c r="N34" s="23" t="s">
         <v>47</v>
@@ -4022,13 +4050,13 @@
         <v>124</v>
       </c>
       <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
+      <c r="M35" s="22" t="s">
+        <v>183</v>
+      </c>
       <c r="N35" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O35" s="24" t="s">
-        <v>183</v>
-      </c>
+      <c r="O35" s="24"/>
     </row>
     <row r="36" spans="1:15" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="17">
@@ -4055,13 +4083,13 @@
         <v>124</v>
       </c>
       <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
+      <c r="M36" s="22" t="s">
+        <v>183</v>
+      </c>
       <c r="N36" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O36" s="24" t="s">
-        <v>183</v>
-      </c>
+      <c r="O36" s="24"/>
     </row>
     <row r="37" spans="1:15" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="17">
@@ -4095,7 +4123,9 @@
         <v>185</v>
       </c>
       <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
+      <c r="L37" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M37" s="22"/>
       <c r="N37" s="23" t="s">
         <v>47</v>
@@ -4127,13 +4157,13 @@
         <v>124</v>
       </c>
       <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
+      <c r="M38" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="N38" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O38" s="24" t="s">
-        <v>180</v>
-      </c>
+      <c r="O38" s="24"/>
     </row>
     <row r="39" spans="1:15" ht="100.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="17">
@@ -4160,13 +4190,13 @@
         <v>124</v>
       </c>
       <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
+      <c r="M39" s="22" t="s">
+        <v>179</v>
+      </c>
       <c r="N39" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O39" s="24" t="s">
-        <v>179</v>
-      </c>
+      <c r="O39" s="24"/>
     </row>
     <row r="40" spans="1:15" ht="84.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17">
@@ -4193,7 +4223,9 @@
         <v>124</v>
       </c>
       <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
+      <c r="M40" s="22" t="s">
+        <v>193</v>
+      </c>
       <c r="N40" s="23" t="s">
         <v>47</v>
       </c>
@@ -4224,13 +4256,13 @@
         <v>124</v>
       </c>
       <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
+      <c r="M41" s="22" t="s">
+        <v>180</v>
+      </c>
       <c r="N41" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O41" s="24" t="s">
-        <v>180</v>
-      </c>
+      <c r="O41" s="24"/>
     </row>
     <row r="42" spans="1:15" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17">
@@ -4257,13 +4289,13 @@
         <v>124</v>
       </c>
       <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
+      <c r="M42" s="22" t="s">
+        <v>181</v>
+      </c>
       <c r="N42" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O42" s="24" t="s">
-        <v>181</v>
-      </c>
+      <c r="O42" s="24"/>
     </row>
     <row r="43" spans="1:15" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17">
@@ -4290,13 +4322,13 @@
         <v>124</v>
       </c>
       <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
+      <c r="M43" s="22" t="s">
+        <v>177</v>
+      </c>
       <c r="N43" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O43" s="24" t="s">
-        <v>177</v>
-      </c>
+      <c r="O43" s="24"/>
     </row>
     <row r="44" spans="1:15" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17">
@@ -4323,13 +4355,13 @@
         <v>124</v>
       </c>
       <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
+      <c r="M44" s="22" t="s">
+        <v>182</v>
+      </c>
       <c r="N44" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O44" s="24" t="s">
-        <v>182</v>
-      </c>
+      <c r="O44" s="24"/>
     </row>
     <row r="45" spans="1:15" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="17">
@@ -4356,13 +4388,13 @@
         <v>124</v>
       </c>
       <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
+      <c r="M45" s="22" t="s">
+        <v>178</v>
+      </c>
       <c r="N45" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O45" s="24" t="s">
-        <v>178</v>
-      </c>
+      <c r="O45" s="24"/>
     </row>
     <row r="46" spans="1:15" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="17">
@@ -4389,13 +4421,13 @@
         <v>124</v>
       </c>
       <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
+      <c r="M46" s="22" t="s">
+        <v>178</v>
+      </c>
       <c r="N46" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O46" s="24" t="s">
-        <v>178</v>
-      </c>
+      <c r="O46" s="24"/>
     </row>
     <row r="47" spans="1:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="17">
@@ -4429,7 +4461,9 @@
         <v>185</v>
       </c>
       <c r="K47" s="22"/>
-      <c r="L47" s="22"/>
+      <c r="L47" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M47" s="22"/>
       <c r="N47" s="23" t="s">
         <v>47</v>
@@ -4468,7 +4502,9 @@
         <v>185</v>
       </c>
       <c r="K48" s="22"/>
-      <c r="L48" s="22"/>
+      <c r="L48" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M48" s="22"/>
       <c r="N48" s="23" t="s">
         <v>47</v>
@@ -4500,13 +4536,13 @@
         <v>124</v>
       </c>
       <c r="L49" s="22"/>
-      <c r="M49" s="22"/>
+      <c r="M49" s="22" t="s">
+        <v>178</v>
+      </c>
       <c r="N49" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O49" s="24" t="s">
-        <v>178</v>
-      </c>
+      <c r="O49" s="24"/>
     </row>
     <row r="50" spans="1:15" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17">
@@ -4533,13 +4569,13 @@
         <v>124</v>
       </c>
       <c r="L50" s="22"/>
-      <c r="M50" s="22"/>
+      <c r="M50" s="22" t="s">
+        <v>178</v>
+      </c>
       <c r="N50" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="O50" s="24" t="s">
-        <v>178</v>
-      </c>
+      <c r="O50" s="24"/>
     </row>
     <row r="51" spans="1:15" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
@@ -4573,7 +4609,9 @@
         <v>185</v>
       </c>
       <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
+      <c r="L51" s="22" t="s">
+        <v>122</v>
+      </c>
       <c r="M51" s="22"/>
       <c r="N51" s="23" t="s">
         <v>47</v>

</xml_diff>